<commit_message>
Revised schedule, sent out for review
</commit_message>
<xml_diff>
--- a/beach-retreat-2016/Beach Retreat Schedule.xlsx
+++ b/beach-retreat-2016/Beach Retreat Schedule.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="34">
   <si>
     <t>Time</t>
   </si>
@@ -120,13 +120,19 @@
   </si>
   <si>
     <t>Lights out</t>
+  </si>
+  <si>
+    <t>Clean-up - ALL</t>
+  </si>
+  <si>
+    <t>Breakfast - ALL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,16 +154,48 @@
       <name val="Matura MT Script Capitals"/>
       <family val="4"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="23">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -268,19 +306,6 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
         <color auto="1"/>
       </left>
       <right style="thin">
@@ -453,7 +478,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -468,7 +493,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -478,37 +502,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF0000"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -789,7 +824,7 @@
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -798,17 +833,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
     </row>
     <row r="2" spans="1:5" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -825,10 +860,10 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="13">
+      <c r="A4" s="12">
         <v>0.312500000000006</v>
       </c>
-      <c r="B4" s="8"/>
+      <c r="B4" s="7"/>
       <c r="C4" s="3" t="s">
         <v>19</v>
       </c>
@@ -840,81 +875,81 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="13">
+      <c r="A5" s="12">
         <v>0.33333333333333898</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="3" t="s">
+      <c r="B5" s="7"/>
+      <c r="C5" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="28" t="s">
         <v>5</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="13">
+      <c r="A6" s="12">
         <v>0.35416666666667201</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="3" t="s">
+      <c r="B6" s="7"/>
+      <c r="C6" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="19" t="s">
-        <v>10</v>
+      <c r="E6" s="17" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="13">
+      <c r="A7" s="12">
         <v>0.375000000000005</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="20" t="s">
+      <c r="B7" s="7"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="13">
+      <c r="A8" s="12">
         <v>0.39583333333333798</v>
       </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="20" t="s">
+      <c r="B8" s="15"/>
+      <c r="C8" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="19" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="13">
+      <c r="A9" s="12">
         <v>0.41666666666667102</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="21" t="s">
+      <c r="B9" s="15"/>
+      <c r="C9" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="16" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="13">
+      <c r="A10" s="12">
         <v>0.437500000000004</v>
       </c>
-      <c r="B10" s="8"/>
+      <c r="B10" s="7"/>
       <c r="C10" s="3" t="s">
         <v>12</v>
       </c>
@@ -926,366 +961,374 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="13">
+      <c r="A11" s="12">
         <v>0.45833333333333598</v>
       </c>
-      <c r="B11" s="8"/>
+      <c r="B11" s="7"/>
       <c r="C11" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="10" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="13">
+      <c r="A12" s="12">
         <v>0.47916666666666902</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>4</v>
+      </c>
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="13">
+      <c r="A13" s="12">
         <v>0.500000000000002</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="3" t="s">
+      <c r="B13" s="7"/>
+      <c r="C13" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="31" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="13">
+      <c r="A14" s="12">
         <v>0.52083333333333504</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="3" t="s">
+      <c r="B14" s="7"/>
+      <c r="C14" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="31" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="13">
+      <c r="A15" s="12">
         <v>0.54166666666666796</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="9" t="s">
+      <c r="B15" s="7"/>
+      <c r="C15" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="9"/>
+      <c r="E15" s="8"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="13">
+      <c r="A16" s="12">
         <v>0.562500000000001</v>
       </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E16" s="10"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="9"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="13">
+      <c r="A17" s="12">
         <v>0.58333333333333404</v>
       </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E17" s="10"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="9"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="13">
+      <c r="A18" s="12">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B18" s="14"/>
-      <c r="C18" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18" s="10"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="9"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="13">
+      <c r="A19" s="12">
         <v>0.625</v>
       </c>
-      <c r="B19" s="14"/>
-      <c r="C19" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E19" s="10"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="9"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="13">
+      <c r="A20" s="12">
         <v>0.64583333333333404</v>
       </c>
-      <c r="B20" s="14"/>
-      <c r="C20" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E20" s="11"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="10"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="13">
+      <c r="A21" s="12">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B21" s="14"/>
-      <c r="C21" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E21" s="10"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="9"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="13">
+      <c r="A22" s="12">
         <v>0.6875</v>
       </c>
-      <c r="B22" s="14"/>
-      <c r="C22" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E22" s="10"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="9"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="13">
+      <c r="A23" s="12">
         <v>0.70833333333333304</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E23" s="11"/>
+      <c r="C23" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="10"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="13">
+      <c r="A24" s="12">
         <v>0.72916666666666696</v>
       </c>
-      <c r="B24" s="14"/>
-      <c r="C24" s="11" t="s">
+      <c r="B24" s="13"/>
+      <c r="C24" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="D24" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E24" s="11"/>
+      <c r="E24" s="10"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="13">
+      <c r="A25" s="12">
         <v>0.75</v>
       </c>
-      <c r="B25" s="14"/>
-      <c r="C25" s="1" t="s">
+      <c r="B25" s="13"/>
+      <c r="C25" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" s="27" t="s">
         <v>13</v>
       </c>
       <c r="E25" s="1"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="13">
+      <c r="A26" s="12">
         <v>0.77083333333333404</v>
       </c>
-      <c r="B26" s="14"/>
-      <c r="C26" s="3" t="s">
+      <c r="B26" s="13"/>
+      <c r="C26" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="26" t="s">
         <v>10</v>
       </c>
       <c r="E26" s="3"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="13">
+      <c r="A27" s="12">
         <v>0.79166666666666696</v>
       </c>
-      <c r="B27" s="14"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="9" t="s">
+      <c r="B27" s="13"/>
+      <c r="C27" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E27" s="9"/>
+      <c r="D27" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="8"/>
     </row>
     <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="13">
+      <c r="A28" s="12">
         <v>0.8125</v>
       </c>
-      <c r="B28" s="14"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E28" s="10"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" s="9"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="13">
+      <c r="A29" s="12">
         <v>0.83333333333333337</v>
       </c>
-      <c r="B29" s="22" t="s">
+      <c r="B29" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C29" s="20" t="s">
+      <c r="C29" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D29" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="E29" s="10"/>
+      <c r="D29" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29" s="9"/>
     </row>
     <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="13">
+      <c r="A30" s="12">
         <v>0.85416666666666663</v>
       </c>
-      <c r="B30" s="22" t="s">
+      <c r="B30" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C30" s="21" t="s">
+      <c r="C30" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="D30" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="E30" s="10"/>
+      <c r="D30" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30" s="9"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="13">
+      <c r="A31" s="12">
         <v>0.875</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="10" t="s">
         <v>4</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D31" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E31" s="10"/>
+      <c r="D31" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E31" s="9"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="13">
+      <c r="A32" s="12">
         <v>0.89583333333333304</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="B32" s="9" t="s">
         <v>14</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D32" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E32" s="10"/>
+      <c r="D32" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E32" s="9"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="13">
+      <c r="A33" s="12">
         <v>0.91666666666666596</v>
       </c>
-      <c r="B33" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C33" s="9" t="s">
+      <c r="B33" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D33" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E33" s="10"/>
+      <c r="D33" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E33" s="9"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="13">
+      <c r="A34" s="12">
         <v>0.937499999999999</v>
       </c>
-      <c r="B34" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D34" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E34" s="10"/>
+      <c r="B34" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E34" s="9"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="13">
+      <c r="A35" s="12">
         <v>0.95833333333333304</v>
       </c>
-      <c r="B35" s="11" t="s">
+      <c r="B35" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D35" s="11" t="s">
+      <c r="D35" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E35" s="11"/>
+      <c r="E35" s="10"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="13">
+      <c r="A36" s="12">
         <v>0.97916666666666596</v>
       </c>
-      <c r="B36" s="11" t="s">
+      <c r="B36" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="C36" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D36" s="11" t="s">
+      <c r="D36" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E36" s="11"/>
+      <c r="E36" s="10"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="26">
+      <c r="A37" s="24">
         <v>0.999999999999999</v>
       </c>
-      <c r="B37" s="15" t="s">
+      <c r="B37" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C37" s="15" t="s">
+      <c r="C37" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="D37" s="15" t="s">
+      <c r="D37" s="14" t="s">
         <v>31</v>
       </c>
       <c r="E37" s="2"/>

</xml_diff>